<commit_message>
Data added Added csv files with data for each prototype associated to a given experiment (Folder).
</commit_message>
<xml_diff>
--- a/07-Plant-Generated-Electricity/Data/Dead-Soil/Dead-Soil.xlsx
+++ b/07-Plant-Generated-Electricity/Data/Dead-Soil/Dead-Soil.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="21">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t xml:space="preserve">DRY+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Night</t>
   </si>
 </sst>
 </file>
@@ -218,8 +239,8 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -934,8 +955,8 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1650,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2368,8 +2389,8 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2383,19 +2404,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2424,7 @@
         <v>44242</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -2455,7 +2476,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -2509,7 +2530,7 @@
         <v>44243</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
@@ -2524,7 +2545,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="n">
         <v>0.85</v>
@@ -2533,7 +2554,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="n">
         <v>0.6</v>
@@ -2542,7 +2563,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="n">
         <v>0.65</v>
@@ -2551,8 +2572,8 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="3" t="n">
         <v>0.48</v>
       </c>
@@ -2561,7 +2582,7 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
@@ -2576,7 +2597,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="n">
         <v>0.02</v>
@@ -2585,7 +2606,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="n">
         <v>0.03</v>
@@ -2594,7 +2615,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="n">
         <v>0.04</v>
@@ -2603,8 +2624,8 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3" t="n">
         <v>0.04</v>
       </c>
@@ -2615,7 +2636,7 @@
         <v>44244</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -2630,7 +2651,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="n">
         <v>0.01</v>
@@ -2639,7 +2660,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="n">
         <v>0.02</v>
@@ -2648,7 +2669,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="n">
         <v>0</v>
@@ -2657,8 +2678,8 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="3" t="n">
         <v>0.01</v>
       </c>
@@ -2667,7 +2688,7 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
@@ -2682,7 +2703,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="n">
         <v>0.01</v>
@@ -2691,7 +2712,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="n">
         <v>0.01</v>
@@ -2700,7 +2721,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="n">
         <v>0.01</v>
@@ -2709,8 +2730,8 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="3" t="n">
         <v>0.01</v>
       </c>
@@ -2720,8 +2741,8 @@
       <c r="A32" s="5" t="n">
         <v>44245</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>5</v>
+      <c r="B32" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>11</v>
@@ -2736,8 +2757,8 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="7" t="n">
         <v>0.03</v>
       </c>
@@ -2745,8 +2766,8 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="7" t="n">
         <v>0.03</v>
       </c>
@@ -2754,8 +2775,8 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="7" t="n">
         <v>0.03</v>
       </c>
@@ -2763,8 +2784,8 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="7" t="n">
         <v>0.05</v>
       </c>
@@ -2772,8 +2793,8 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="B37" s="6" t="s">
-        <v>7</v>
+      <c r="B37" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>11</v>
@@ -2788,8 +2809,8 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="7" t="n">
         <v>0.03</v>
       </c>
@@ -2797,8 +2818,8 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="7" t="n">
         <v>0.01</v>
       </c>
@@ -2806,8 +2827,8 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="7" t="n">
         <v>0.01</v>
       </c>
@@ -2815,8 +2836,8 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="6"/>
       <c r="D41" s="7" t="n">
         <v>0.04</v>
       </c>
@@ -2826,8 +2847,8 @@
       <c r="A42" s="5" t="n">
         <v>44246</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>5</v>
+      <c r="B42" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>9</v>
@@ -2842,8 +2863,8 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="6"/>
       <c r="D43" s="7" t="n">
         <v>0.58</v>
       </c>
@@ -2851,8 +2872,8 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="6"/>
       <c r="D44" s="7" t="n">
         <v>0.72</v>
       </c>
@@ -2860,8 +2881,8 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="6"/>
       <c r="D45" s="7" t="n">
         <v>0.63</v>
       </c>
@@ -2869,8 +2890,8 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="6"/>
       <c r="D46" s="7" t="n">
         <v>0.88</v>
       </c>
@@ -2878,8 +2899,8 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
-      <c r="B47" s="6" t="s">
-        <v>7</v>
+      <c r="B47" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>12</v>
@@ -2894,8 +2915,8 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="6"/>
       <c r="D48" s="7" t="n">
         <v>0.26</v>
       </c>
@@ -2903,8 +2924,8 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="6"/>
       <c r="D49" s="7" t="n">
         <v>0.3</v>
       </c>
@@ -2912,8 +2933,8 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="6"/>
       <c r="D50" s="7" t="n">
         <v>0.26</v>
       </c>
@@ -2921,8 +2942,8 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="6"/>
       <c r="D51" s="7" t="n">
         <v>0.26</v>
       </c>
@@ -2932,8 +2953,8 @@
       <c r="A52" s="5" t="n">
         <v>44247</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>5</v>
+      <c r="B52" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>10</v>
@@ -2948,8 +2969,8 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="6"/>
       <c r="D53" s="7" t="n">
         <v>0.14</v>
       </c>
@@ -2957,8 +2978,8 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="6"/>
       <c r="D54" s="7" t="n">
         <v>0.15</v>
       </c>
@@ -2966,8 +2987,8 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="6"/>
       <c r="D55" s="7" t="n">
         <v>0.07</v>
       </c>
@@ -2975,8 +2996,8 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="6"/>
       <c r="D56" s="7" t="n">
         <v>0.14</v>
       </c>
@@ -2984,8 +3005,8 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
-      <c r="B57" s="6" t="s">
-        <v>7</v>
+      <c r="B57" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>11</v>
@@ -2998,29 +3019,29 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="6"/>
       <c r="D58" s="1"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="6"/>
       <c r="D59" s="1"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="6"/>
       <c r="D60" s="1"/>
       <c r="E60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="6"/>
       <c r="D61" s="1"/>
       <c r="E61" s="8"/>
     </row>
@@ -3087,7 +3108,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>